<commit_message>
excell okuyan kod eklendi
</commit_message>
<xml_diff>
--- a/GeneticAlgorithm/datasheet.xlsx
+++ b/GeneticAlgorithm/datasheet.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgeler\workspace\vscode\cs125\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Excalibur-\Desktop\ScheduleMaker\GeneticAlgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B3D8BC-4139-40F2-9EC0-396FCD573099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOMS" sheetId="1" r:id="rId1"/>
     <sheet name="MEETING_TIMES" sheetId="2" r:id="rId2"/>
     <sheet name="INSTRUCTORS" sheetId="3" r:id="rId3"/>
     <sheet name="COURSES" sheetId="4" r:id="rId4"/>
+    <sheet name="Sayfa1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>R1</t>
   </si>
@@ -124,12 +126,24 @@
   </si>
   <si>
     <t>EE</t>
+  </si>
+  <si>
+    <t>anam</t>
+  </si>
+  <si>
+    <t>babam</t>
+  </si>
+  <si>
+    <t>cnm</t>
+  </si>
+  <si>
+    <t>benim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -947,10 +961,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -986,7 +1000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1033,7 +1047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1092,7 +1106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1202,4 +1216,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41DAA90-966A-4ECA-A9D6-CF41782F7C3B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>